<commit_message>
add org drop down list into Muliple User Template file
</commit_message>
<xml_diff>
--- a/Presentation/wwwroot/files/Multiple Users Template.xlsx
+++ b/Presentation/wwwroot/files/Multiple Users Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim.radi.FLAIRSTECH\source\repos\Flairstech\SchoolsManagementSystem\Presentation\wwwroot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0A259F-AC32-47BB-9CB9-16ECFC836639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7207904-3E0D-4820-8FC1-8D35E2C56C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>MotherMobile (Optional)</t>
+  </si>
+  <si>
+    <t>Email (Optional)</t>
   </si>
 </sst>
 </file>
@@ -434,12 +434,12 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
@@ -457,46 +457,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assign bulk of class members when add users bulk
</commit_message>
<xml_diff>
--- a/Presentation/wwwroot/files/Multiple Users Template.xlsx
+++ b/Presentation/wwwroot/files/Multiple Users Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim.radi.FLAIRSTECH\source\repos\Flairstech\SchoolsManagementSystem\Presentation\wwwroot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7207904-3E0D-4820-8FC1-8D35E2C56C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1BB035-A8E9-4187-873E-1CE6BB6BC455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Organizations (Optional)</t>
   </si>
   <si>
     <t>Address (Optional)</t>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,17 +452,17 @@
     <col min="14" max="14" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -483,7 +480,7 @@
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="4" t="s">
@@ -494,9 +491,6 @@
       </c>
       <c r="M1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>